<commit_message>
Updated FER analysis for CFO
</commit_message>
<xml_diff>
--- a/utils/FER_S1G_Analysis.xlsx
+++ b/utils/FER_S1G_Analysis.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="110">
+  <si>
+    <t>CFO: 0 kHz</t>
+  </si>
   <si>
     <t>Frame Error Rate (FER)</t>
   </si>
@@ -49,16 +52,16 @@
     <t>MCS 8</t>
   </si>
   <si>
-    <t>0.813</t>
-  </si>
-  <si>
-    <t>0.289</t>
-  </si>
-  <si>
-    <t>0.035</t>
-  </si>
-  <si>
-    <t>0.0025</t>
+    <t>0.8064</t>
+  </si>
+  <si>
+    <t>0.306</t>
+  </si>
+  <si>
+    <t>0.0349</t>
+  </si>
+  <si>
+    <t>0.00255</t>
   </si>
   <si>
     <t>0.966</t>
@@ -67,127 +70,280 @@
     <t>XX</t>
   </si>
   <si>
-    <t>0.656</t>
-  </si>
-  <si>
-    <t>0.251</t>
-  </si>
-  <si>
-    <t>0.971</t>
-  </si>
-  <si>
-    <t>0.070</t>
-  </si>
-  <si>
-    <t>0.680</t>
-  </si>
-  <si>
-    <t>0.010</t>
-  </si>
-  <si>
-    <t>0.272</t>
-  </si>
-  <si>
-    <t>0.056</t>
+    <t>0.660</t>
+  </si>
+  <si>
+    <t>0.255</t>
+  </si>
+  <si>
+    <t>0.9615</t>
+  </si>
+  <si>
+    <t>0.0689</t>
+  </si>
+  <si>
+    <t>0.692</t>
+  </si>
+  <si>
+    <t>0.0099</t>
+  </si>
+  <si>
+    <t>0.267</t>
+  </si>
+  <si>
+    <t>0.0548</t>
   </si>
   <si>
     <t>0.006</t>
   </si>
   <si>
-    <t>0.922</t>
-  </si>
-  <si>
-    <t>0.536</t>
-  </si>
-  <si>
-    <t>0.156</t>
+    <t>0.9216</t>
+  </si>
+  <si>
+    <t>0.5319</t>
+  </si>
+  <si>
+    <t>0.151</t>
   </si>
   <si>
     <t>0.041</t>
   </si>
   <si>
-    <t>0.855</t>
+    <t>0.862</t>
+  </si>
+  <si>
+    <t>0.0075</t>
+  </si>
+  <si>
+    <t>0.4514</t>
+  </si>
+  <si>
+    <t>0.1367</t>
+  </si>
+  <si>
+    <t>0.030</t>
+  </si>
+  <si>
+    <t>0.0053</t>
+  </si>
+  <si>
+    <t>0.985</t>
+  </si>
+  <si>
+    <t>0.990</t>
+  </si>
+  <si>
+    <t>0.2849</t>
+  </si>
+  <si>
+    <t>0.7575</t>
+  </si>
+  <si>
+    <t>0.0874</t>
+  </si>
+  <si>
+    <t>0.3448</t>
+  </si>
+  <si>
+    <t>0.8547</t>
+  </si>
+  <si>
+    <t>0.0187</t>
+  </si>
+  <si>
+    <t>0.1058</t>
+  </si>
+  <si>
+    <t>0.475</t>
+  </si>
+  <si>
+    <t>0.00346</t>
+  </si>
+  <si>
+    <t>0.023</t>
+  </si>
+  <si>
+    <t>0.1874</t>
+  </si>
+  <si>
+    <t>0.00429</t>
+  </si>
+  <si>
+    <t>0.0515</t>
+  </si>
+  <si>
+    <t>0.011</t>
+  </si>
+  <si>
+    <t>0.9174</t>
+  </si>
+  <si>
+    <t>0.0022</t>
+  </si>
+  <si>
+    <t>0.5602</t>
+  </si>
+  <si>
+    <t>0.2567</t>
+  </si>
+  <si>
+    <t>0.0693</t>
+  </si>
+  <si>
+    <t>0.0166</t>
+  </si>
+  <si>
+    <t>0.0034</t>
+  </si>
+  <si>
+    <t>CFO: 25 kHz</t>
+  </si>
+  <si>
+    <t>0.378</t>
+  </si>
+  <si>
+    <t>0.0737</t>
   </si>
   <si>
     <t>0.008</t>
   </si>
   <si>
-    <t>0.449</t>
-  </si>
-  <si>
-    <t>0.138</t>
-  </si>
-  <si>
-    <t>0.030</t>
-  </si>
-  <si>
-    <t>0.005</t>
-  </si>
-  <si>
-    <t>0.976</t>
-  </si>
-  <si>
-    <t>0.699</t>
-  </si>
-  <si>
-    <t>0.990</t>
-  </si>
-  <si>
-    <t>0.291</t>
-  </si>
-  <si>
-    <t>0.760</t>
-  </si>
-  <si>
-    <t>0.087</t>
-  </si>
-  <si>
-    <t>0.354</t>
-  </si>
-  <si>
-    <t>0.877</t>
-  </si>
-  <si>
-    <t>0.020</t>
-  </si>
-  <si>
-    <t>0.105</t>
-  </si>
-  <si>
-    <t>0.485</t>
-  </si>
-  <si>
-    <t>0.004</t>
-  </si>
-  <si>
-    <t>0.024</t>
-  </si>
-  <si>
-    <t>0.193</t>
-  </si>
-  <si>
-    <t>0.053</t>
-  </si>
-  <si>
-    <t>0.012</t>
-  </si>
-  <si>
-    <t>0.935</t>
-  </si>
-  <si>
-    <t>0.002</t>
-  </si>
-  <si>
-    <t>0.573</t>
-  </si>
-  <si>
-    <t>0.256</t>
-  </si>
-  <si>
-    <t>0.071</t>
-  </si>
-  <si>
-    <t>0.018</t>
+    <t>0.98039</t>
+  </si>
+  <si>
+    <t>0.7017</t>
+  </si>
+  <si>
+    <t>0.3257</t>
+  </si>
+  <si>
+    <t>0.0987</t>
+  </si>
+  <si>
+    <t>0.75188</t>
+  </si>
+  <si>
+    <t>0.01739</t>
+  </si>
+  <si>
+    <t>0.30165</t>
+  </si>
+  <si>
+    <t>0.07532</t>
+  </si>
+  <si>
+    <t>0.01155</t>
+  </si>
+  <si>
+    <t>0.61349</t>
+  </si>
+  <si>
+    <t>0.20682</t>
+  </si>
+  <si>
+    <t>0.05506</t>
+  </si>
+  <si>
+    <t>0.9259</t>
+  </si>
+  <si>
+    <t>0.01133</t>
+  </si>
+  <si>
+    <t>0.542</t>
+  </si>
+  <si>
+    <t>0.20141</t>
+  </si>
+  <si>
+    <t>0.04927</t>
+  </si>
+  <si>
+    <t>0.00786</t>
+  </si>
+  <si>
+    <t>0.85106</t>
+  </si>
+  <si>
+    <t>0.995</t>
+  </si>
+  <si>
+    <t>0.44943</t>
+  </si>
+  <si>
+    <t>0.88495</t>
+  </si>
+  <si>
+    <t>0.16103</t>
+  </si>
+  <si>
+    <t>0.5154</t>
+  </si>
+  <si>
+    <t>0.9756</t>
+  </si>
+  <si>
+    <t>0.03810</t>
+  </si>
+  <si>
+    <t>0.1974</t>
+  </si>
+  <si>
+    <t>0.00984</t>
+  </si>
+  <si>
+    <t>0.0665</t>
+  </si>
+  <si>
+    <t>0.3597</t>
+  </si>
+  <si>
+    <t>0.0196</t>
+  </si>
+  <si>
+    <t>0.14749</t>
+  </si>
+  <si>
+    <t>0.04292</t>
+  </si>
+  <si>
+    <t>0.01238</t>
+  </si>
+  <si>
+    <t>0.94339</t>
+  </si>
+  <si>
+    <t>0.70422</t>
+  </si>
+  <si>
+    <t>0.41322</t>
+  </si>
+  <si>
+    <t>0.19627</t>
+  </si>
+  <si>
+    <t>0.08822</t>
+  </si>
+  <si>
+    <t>SNR of SDR Impl.</t>
+  </si>
+  <si>
+    <t>Tx</t>
+  </si>
+  <si>
+    <t>Rx</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.6</t>
   </si>
 </sst>
 </file>
@@ -195,10 +351,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -217,14 +373,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -233,7 +381,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,18 +426,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -272,22 +481,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,59 +511,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -376,7 +532,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,7 +556,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,19 +580,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,7 +622,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,49 +682,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,55 +694,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,30 +858,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -737,30 +869,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -799,153 +907,201 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -953,7 +1109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -980,18 +1136,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1010,10 +1163,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1335,18 +1491,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="H44" workbookViewId="0">
+      <selection activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" ht="13.5" spans="1:11">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1355,41 +1513,41 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" ht="13.5" spans="1:11">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="16"/>
+      <c r="J2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="6">
@@ -1419,10 +1577,10 @@
       <c r="I3" s="7">
         <v>1</v>
       </c>
-      <c r="J3" s="18">
-        <v>1</v>
-      </c>
-      <c r="K3" s="16"/>
+      <c r="J3" s="17">
+        <v>1</v>
+      </c>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="8">
@@ -1452,17 +1610,17 @@
       <c r="I4" s="9">
         <v>1</v>
       </c>
-      <c r="J4" s="19">
-        <v>1</v>
-      </c>
-      <c r="K4" s="16"/>
+      <c r="J4" s="18">
+        <v>1</v>
+      </c>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="8">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="9">
         <v>1</v>
@@ -1485,17 +1643,17 @@
       <c r="I5" s="9">
         <v>1</v>
       </c>
-      <c r="J5" s="19">
-        <v>1</v>
-      </c>
-      <c r="K5" s="16"/>
+      <c r="J5" s="18">
+        <v>1</v>
+      </c>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="8">
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" s="9">
         <v>1</v>
@@ -1518,17 +1676,17 @@
       <c r="I6" s="9">
         <v>1</v>
       </c>
-      <c r="J6" s="19">
-        <v>1</v>
-      </c>
-      <c r="K6" s="16"/>
+      <c r="J6" s="18">
+        <v>1</v>
+      </c>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="8">
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -1551,20 +1709,20 @@
       <c r="I7" s="9">
         <v>1</v>
       </c>
-      <c r="J7" s="19">
-        <v>1</v>
-      </c>
-      <c r="K7" s="16"/>
+      <c r="J7" s="18">
+        <v>1</v>
+      </c>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="8">
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
@@ -1584,20 +1742,20 @@
       <c r="I8" s="9">
         <v>1</v>
       </c>
-      <c r="J8" s="19">
-        <v>1</v>
-      </c>
-      <c r="K8" s="16"/>
+      <c r="J8" s="18">
+        <v>1</v>
+      </c>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="8">
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="9">
         <v>1</v>
@@ -1617,23 +1775,23 @@
       <c r="I9" s="9">
         <v>1</v>
       </c>
-      <c r="J9" s="19">
-        <v>1</v>
-      </c>
-      <c r="K9" s="16"/>
+      <c r="J9" s="18">
+        <v>1</v>
+      </c>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="8">
         <v>7</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E10" s="9">
         <v>1</v>
@@ -1650,23 +1808,23 @@
       <c r="I10" s="9">
         <v>1</v>
       </c>
-      <c r="J10" s="19">
-        <v>1</v>
-      </c>
-      <c r="K10" s="16"/>
+      <c r="J10" s="18">
+        <v>1</v>
+      </c>
+      <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="8">
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E11" s="9">
         <v>1</v>
@@ -1683,23 +1841,23 @@
       <c r="I11" s="9">
         <v>1</v>
       </c>
-      <c r="J11" s="19">
-        <v>1</v>
-      </c>
-      <c r="K11" s="16"/>
+      <c r="J11" s="18">
+        <v>1</v>
+      </c>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="8">
         <v>9</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="9">
         <v>1</v>
@@ -1716,23 +1874,23 @@
       <c r="I12" s="9">
         <v>1</v>
       </c>
-      <c r="J12" s="19">
-        <v>1</v>
-      </c>
-      <c r="K12" s="16"/>
+      <c r="J12" s="18">
+        <v>1</v>
+      </c>
+      <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="8">
         <v>10</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="9">
         <v>1</v>
@@ -1749,26 +1907,26 @@
       <c r="I13" s="9">
         <v>1</v>
       </c>
-      <c r="J13" s="19">
-        <v>1</v>
-      </c>
-      <c r="K13" s="16"/>
+      <c r="J13" s="18">
+        <v>1</v>
+      </c>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="8">
         <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F14" s="9">
         <v>1</v>
@@ -1782,26 +1940,26 @@
       <c r="I14" s="9">
         <v>1</v>
       </c>
-      <c r="J14" s="19">
-        <v>1</v>
-      </c>
-      <c r="K14" s="16"/>
+      <c r="J14" s="18">
+        <v>1</v>
+      </c>
+      <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="8">
         <v>12</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F15" s="9">
         <v>1</v>
@@ -1815,26 +1973,26 @@
       <c r="I15" s="9">
         <v>1</v>
       </c>
-      <c r="J15" s="19">
-        <v>1</v>
-      </c>
-      <c r="K15" s="16"/>
+      <c r="J15" s="18">
+        <v>1</v>
+      </c>
+      <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="8">
         <v>13</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F16" s="9">
         <v>1</v>
@@ -1848,29 +2006,29 @@
       <c r="I16" s="9">
         <v>1</v>
       </c>
-      <c r="J16" s="19">
-        <v>1</v>
-      </c>
-      <c r="K16" s="16"/>
+      <c r="J16" s="18">
+        <v>1</v>
+      </c>
+      <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="8">
         <v>14</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G17" s="9">
         <v>1</v>
@@ -1881,29 +2039,29 @@
       <c r="I17" s="9">
         <v>1</v>
       </c>
-      <c r="J17" s="19">
-        <v>1</v>
-      </c>
-      <c r="K17" s="16"/>
+      <c r="J17" s="18">
+        <v>1</v>
+      </c>
+      <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="8">
         <v>15</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G18" s="9">
         <v>1</v>
@@ -1914,29 +2072,29 @@
       <c r="I18" s="9">
         <v>1</v>
       </c>
-      <c r="J18" s="19">
-        <v>1</v>
-      </c>
-      <c r="K18" s="16"/>
+      <c r="J18" s="18">
+        <v>1</v>
+      </c>
+      <c r="K18" s="15"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="8">
         <v>16</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G19" s="9">
         <v>1</v>
@@ -1947,29 +2105,29 @@
       <c r="I19" s="9">
         <v>1</v>
       </c>
-      <c r="J19" s="19">
-        <v>1</v>
-      </c>
-      <c r="K19" s="16"/>
+      <c r="J19" s="18">
+        <v>1</v>
+      </c>
+      <c r="K19" s="15"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="10">
+      <c r="A20" s="8">
         <v>17</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G20" s="9">
         <v>1</v>
@@ -1980,32 +2138,32 @@
       <c r="I20" s="9">
         <v>1</v>
       </c>
-      <c r="J20" s="19">
-        <v>1</v>
-      </c>
-      <c r="K20" s="16"/>
+      <c r="J20" s="18">
+        <v>1</v>
+      </c>
+      <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="10">
+      <c r="A21" s="8">
         <v>18</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H21" s="9">
         <v>1</v>
@@ -2013,32 +2171,32 @@
       <c r="I21" s="9">
         <v>1</v>
       </c>
-      <c r="J21" s="19">
-        <v>1</v>
-      </c>
-      <c r="K21" s="16"/>
+      <c r="J21" s="18">
+        <v>1</v>
+      </c>
+      <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="10">
+      <c r="A22" s="8">
         <v>19</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>38</v>
@@ -2046,127 +2204,127 @@
       <c r="I22" s="9">
         <v>1</v>
       </c>
-      <c r="J22" s="19">
-        <v>1</v>
-      </c>
-      <c r="K22" s="16"/>
+      <c r="J22" s="18">
+        <v>1</v>
+      </c>
+      <c r="K22" s="15"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="11">
+      <c r="A23" s="8">
         <v>20</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="J23" s="19">
-        <v>1</v>
-      </c>
-      <c r="K23" s="16"/>
+      <c r="J23" s="18">
+        <v>1</v>
+      </c>
+      <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="10">
+      <c r="A24" s="8">
         <v>21</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="J24" s="19">
-        <v>1</v>
-      </c>
-      <c r="K24" s="16"/>
+      <c r="J24" s="18">
+        <v>1</v>
+      </c>
+      <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="10">
+      <c r="A25" s="8">
         <v>22</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J25" s="19">
+      <c r="J25" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="11">
+      <c r="A26" s="8">
         <v>23</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>47</v>
@@ -2174,42 +2332,42 @@
       <c r="H26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I26" s="14" t="s">
+      <c r="I26" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="J26" s="19">
+      <c r="J26" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="10">
+      <c r="A27" s="8">
         <v>24</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G27" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J27" s="19">
+        <v>51</v>
+      </c>
+      <c r="J27" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2218,31 +2376,31 @@
         <v>25</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J28" s="19" t="s">
         <v>52</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -2250,31 +2408,31 @@
         <v>26</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J29" s="19" t="s">
         <v>54</v>
+      </c>
+      <c r="J29" s="18" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -2282,31 +2440,31 @@
         <v>27</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I30" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J30" s="19" t="s">
-        <v>55</v>
+        <v>17</v>
+      </c>
+      <c r="J30" s="18" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -2314,31 +2472,31 @@
         <v>28</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J31" s="19" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="J31" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -2346,31 +2504,31 @@
         <v>29</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J32" s="19" t="s">
-        <v>57</v>
+        <v>17</v>
+      </c>
+      <c r="J32" s="18" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -2378,74 +2536,1461 @@
         <v>30</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" ht="13.5" spans="1:10">
+      <c r="A34" s="10">
+        <v>31</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" ht="13.5"/>
+    <row r="38" ht="13.5" spans="1:10">
+      <c r="A38" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" ht="13.5" spans="1:10">
+      <c r="A39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="6">
+        <v>0</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1</v>
+      </c>
+      <c r="C40" s="7">
+        <v>1</v>
+      </c>
+      <c r="D40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+      <c r="G40" s="7">
+        <v>1</v>
+      </c>
+      <c r="H40" s="7">
+        <v>1</v>
+      </c>
+      <c r="I40" s="7">
+        <v>1</v>
+      </c>
+      <c r="J40" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="8">
+        <v>1</v>
+      </c>
+      <c r="B41" s="9">
+        <v>1</v>
+      </c>
+      <c r="C41" s="9">
+        <v>1</v>
+      </c>
+      <c r="D41" s="9">
+        <v>1</v>
+      </c>
+      <c r="E41" s="9">
+        <v>1</v>
+      </c>
+      <c r="F41" s="9">
+        <v>1</v>
+      </c>
+      <c r="G41" s="9">
+        <v>1</v>
+      </c>
+      <c r="H41" s="9">
+        <v>1</v>
+      </c>
+      <c r="I41" s="9">
+        <v>1</v>
+      </c>
+      <c r="J41" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="8">
+        <v>2</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="9">
+        <v>1</v>
+      </c>
+      <c r="D42" s="9">
+        <v>1</v>
+      </c>
+      <c r="E42" s="9">
+        <v>1</v>
+      </c>
+      <c r="F42" s="9">
+        <v>1</v>
+      </c>
+      <c r="G42" s="9">
+        <v>1</v>
+      </c>
+      <c r="H42" s="9">
+        <v>1</v>
+      </c>
+      <c r="I42" s="9">
+        <v>1</v>
+      </c>
+      <c r="J42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="8">
+        <v>3</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="9">
+        <v>1</v>
+      </c>
+      <c r="D43" s="9">
+        <v>1</v>
+      </c>
+      <c r="E43" s="9">
+        <v>1</v>
+      </c>
+      <c r="F43" s="9">
+        <v>1</v>
+      </c>
+      <c r="G43" s="9">
+        <v>1</v>
+      </c>
+      <c r="H43" s="9">
+        <v>1</v>
+      </c>
+      <c r="I43" s="9">
+        <v>1</v>
+      </c>
+      <c r="J43" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="8">
+        <v>4</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+      <c r="D44" s="9">
+        <v>1</v>
+      </c>
+      <c r="E44" s="9">
+        <v>1</v>
+      </c>
+      <c r="F44" s="9">
+        <v>1</v>
+      </c>
+      <c r="G44" s="9">
+        <v>1</v>
+      </c>
+      <c r="H44" s="9">
+        <v>1</v>
+      </c>
+      <c r="I44" s="9">
+        <v>1</v>
+      </c>
+      <c r="J44" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="8">
+        <v>5</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="9">
+        <v>1</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1</v>
+      </c>
+      <c r="F45" s="9">
+        <v>1</v>
+      </c>
+      <c r="G45" s="9">
+        <v>1</v>
+      </c>
+      <c r="H45" s="9">
+        <v>1</v>
+      </c>
+      <c r="I45" s="9">
+        <v>1</v>
+      </c>
+      <c r="J45" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="8">
+        <v>6</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="9">
+        <v>1</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
+      <c r="F46" s="9">
+        <v>1</v>
+      </c>
+      <c r="G46" s="9">
+        <v>1</v>
+      </c>
+      <c r="H46" s="9">
+        <v>1</v>
+      </c>
+      <c r="I46" s="9">
+        <v>1</v>
+      </c>
+      <c r="J46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="8">
+        <v>7</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="F47" s="9">
+        <v>1</v>
+      </c>
+      <c r="G47" s="9">
+        <v>1</v>
+      </c>
+      <c r="H47" s="9">
+        <v>1</v>
+      </c>
+      <c r="I47" s="9">
+        <v>1</v>
+      </c>
+      <c r="J47" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="8">
+        <v>8</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="9">
+        <v>1</v>
+      </c>
+      <c r="F48" s="9">
+        <v>1</v>
+      </c>
+      <c r="G48" s="9">
+        <v>1</v>
+      </c>
+      <c r="H48" s="9">
+        <v>1</v>
+      </c>
+      <c r="I48" s="9">
+        <v>1</v>
+      </c>
+      <c r="J48" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="8">
+        <v>9</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="9">
+        <v>1</v>
+      </c>
+      <c r="F49" s="9">
+        <v>1</v>
+      </c>
+      <c r="G49" s="9">
+        <v>1</v>
+      </c>
+      <c r="H49" s="9">
+        <v>1</v>
+      </c>
+      <c r="I49" s="9">
+        <v>1</v>
+      </c>
+      <c r="J49" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="8">
+        <v>10</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" s="9">
+        <v>1</v>
+      </c>
+      <c r="F50" s="9">
+        <v>1</v>
+      </c>
+      <c r="G50" s="9">
+        <v>1</v>
+      </c>
+      <c r="H50" s="9">
+        <v>1</v>
+      </c>
+      <c r="I50" s="9">
+        <v>1</v>
+      </c>
+      <c r="J50" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="8">
+        <v>11</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="9">
+        <v>1</v>
+      </c>
+      <c r="G51" s="9">
+        <v>1</v>
+      </c>
+      <c r="H51" s="9">
+        <v>1</v>
+      </c>
+      <c r="I51" s="9">
+        <v>1</v>
+      </c>
+      <c r="J51" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="8">
+        <v>12</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52" s="9">
+        <v>1</v>
+      </c>
+      <c r="G52" s="9">
+        <v>1</v>
+      </c>
+      <c r="H52" s="9">
+        <v>1</v>
+      </c>
+      <c r="I52" s="9">
+        <v>1</v>
+      </c>
+      <c r="J52" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="8">
+        <v>13</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="9">
+        <v>1</v>
+      </c>
+      <c r="G53" s="9">
+        <v>1</v>
+      </c>
+      <c r="H53" s="9">
+        <v>1</v>
+      </c>
+      <c r="I53" s="9">
+        <v>1</v>
+      </c>
+      <c r="J53" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="8">
+        <v>14</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G54" s="9">
+        <v>1</v>
+      </c>
+      <c r="H54" s="9">
+        <v>1</v>
+      </c>
+      <c r="I54" s="9">
+        <v>1</v>
+      </c>
+      <c r="J54" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="8">
+        <v>15</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" s="9">
+        <v>1</v>
+      </c>
+      <c r="H55" s="9">
+        <v>1</v>
+      </c>
+      <c r="I55" s="9">
+        <v>1</v>
+      </c>
+      <c r="J55" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="8">
         <v>16</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" ht="13.5" spans="1:10">
-      <c r="A34" s="12">
+      <c r="B56" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" s="9">
+        <v>1</v>
+      </c>
+      <c r="H56" s="9">
+        <v>1</v>
+      </c>
+      <c r="I56" s="9">
+        <v>1</v>
+      </c>
+      <c r="J56" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="8">
+        <v>17</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G57" s="9">
+        <v>1</v>
+      </c>
+      <c r="H57" s="9">
+        <v>1</v>
+      </c>
+      <c r="I57" s="9">
+        <v>1</v>
+      </c>
+      <c r="J57" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="8">
+        <v>18</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G58" s="9">
+        <v>1</v>
+      </c>
+      <c r="H58" s="9">
+        <v>1</v>
+      </c>
+      <c r="I58" s="9">
+        <v>1</v>
+      </c>
+      <c r="J58" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="8">
+        <v>19</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="I59" s="9">
+        <v>1</v>
+      </c>
+      <c r="J59" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="8">
+        <v>20</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="J60" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="8">
+        <v>21</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="J61" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="8">
+        <v>22</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J62" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="8">
+        <v>23</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="J63" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="8">
+        <v>24</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J64" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="8">
+        <v>25</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="J65" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="8">
+        <v>26</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="J66" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="8">
+        <v>27</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I67" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J67" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="8">
+        <v>28</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I68" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J68" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="8">
+        <v>29</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G69" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H69" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J69" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="8">
+        <v>30</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G70" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I70" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J70" s="18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71" ht="13.5" spans="1:10">
+      <c r="A71" s="10">
         <v>31</v>
       </c>
-      <c r="B34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="J34" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="69" spans="5:8">
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
+      <c r="B71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J71" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C76" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77">
+        <v>1</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D77" s="21">
+        <v>40335</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78">
+        <v>2</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C78" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D78" s="21">
+        <v>42077</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C79" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D79" s="21">
+        <v>41975</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80">
+        <v>4</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C80" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D80" s="21">
+        <v>38629</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81">
+        <v>5</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C81" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D81" s="21">
+        <v>36516</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82">
+        <v>6</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D82" s="21">
+        <v>38683</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83">
+        <v>7</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D83" s="21">
+        <v>42698</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84">
+        <v>8</v>
+      </c>
+      <c r="B84" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D84" s="21">
+        <v>39131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85">
+        <v>9</v>
+      </c>
+      <c r="B85" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C85" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D85" s="21">
+        <v>36044</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86">
+        <v>10</v>
+      </c>
+      <c r="B86" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C86" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D86" s="21">
+        <v>41471</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4">
+      <c r="D87">
+        <f>SUM(D77:D86)/10/1000</f>
+        <v>39.7559</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="C89" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="D89" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90">
+        <v>1</v>
+      </c>
+      <c r="B90" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C90" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D90" s="21">
+        <v>38205</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91">
+        <v>2</v>
+      </c>
+      <c r="B91" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D91" s="21">
+        <v>38344</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92">
+        <v>3</v>
+      </c>
+      <c r="B92" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C92" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D92" s="21">
+        <v>38755</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>4</v>
+      </c>
+      <c r="B93" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C93" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D93" s="21">
+        <v>41316</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>5</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C94" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D94" s="21">
+        <v>40710</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>6</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C95" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D95" s="21">
+        <v>42358</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>7</v>
+      </c>
+      <c r="B96" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C96" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D96" s="21">
+        <v>35712</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>8</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C97" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D97" s="21">
+        <v>38505</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98">
+        <v>9</v>
+      </c>
+      <c r="B98" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C98" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D98" s="21">
+        <v>30665</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99">
+        <v>10</v>
+      </c>
+      <c r="B99" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C99" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D99" s="21">
+        <v>33885</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4">
+      <c r="D100">
+        <f>SUM(D90:D99)/10/1000</f>
+        <v>37.8455</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B38:J38"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Added SDR test results
</commit_message>
<xml_diff>
--- a/utils/FER_S1G_Analysis.xlsx
+++ b/utils/FER_S1G_Analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="265">
   <si>
     <t>CFO: 0 ppm | SFO: 0 ppm</t>
   </si>
@@ -766,25 +766,49 @@
     <t>0.2902</t>
   </si>
   <si>
-    <t>SNR of SDR Impl.</t>
-  </si>
-  <si>
-    <t>Tx</t>
-  </si>
-  <si>
-    <t>Rx</t>
-  </si>
-  <si>
-    <t>SNR</t>
-  </si>
-  <si>
-    <t>0.75</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.6</t>
+    <t>Indoor SDR Test</t>
+  </si>
+  <si>
+    <t>AVG SNR [dB]</t>
+  </si>
+  <si>
+    <t>35,095?</t>
+  </si>
+  <si>
+    <t>SUCCSESS</t>
+  </si>
+  <si>
+    <t>ERRORS</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>FER</t>
+  </si>
+  <si>
+    <t>Duration [min]</t>
+  </si>
+  <si>
+    <t>Tx Gain</t>
+  </si>
+  <si>
+    <t>Rx Gain</t>
+  </si>
+  <si>
+    <t>Amp Factor</t>
+  </si>
+  <si>
+    <t>MSG Period [ms]</t>
+  </si>
+  <si>
+    <t>PDU Length [Byte]</t>
+  </si>
+  <si>
+    <t>LO Offset [MHz]</t>
+  </si>
+  <si>
+    <t>Center Freq. [MHz]</t>
   </si>
 </sst>
 </file>
@@ -1152,7 +1176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1299,6 +1323,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1431,7 +1466,7 @@
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1473,10 +1508,10 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1485,28 +1520,28 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1527,13 +1562,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1546,7 +1581,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1604,11 +1639,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1929,13 +1997,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AS100"/>
+  <dimension ref="A1:AS108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AL14" sqref="AL14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="16.6933333333333" customWidth="1"/>
+    <col min="2" max="3" width="12.5"/>
+    <col min="7" max="7" width="9.8"/>
+  </cols>
   <sheetData>
     <row r="1" ht="13.5" spans="1:39">
       <c r="A1" s="1" t="s">
@@ -8177,327 +8250,720 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
+    <row r="74" ht="13.5" spans="1:3">
+      <c r="A74" s="19" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="76" spans="2:4">
-      <c r="B76" s="19" t="s">
+      <c r="B74" s="19"/>
+      <c r="C74" s="19"/>
+    </row>
+    <row r="75" ht="13.5" spans="2:10">
+      <c r="B75" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="14"/>
+    </row>
+    <row r="76" ht="13.5" spans="1:10">
+      <c r="A76" s="4"/>
+      <c r="B76" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H76" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J76" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" ht="13.5" spans="1:10">
+      <c r="A77" s="20" t="s">
         <v>251</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="B77" s="21">
+        <v>30.219</v>
+      </c>
+      <c r="C77" s="22">
+        <v>30.25</v>
+      </c>
+      <c r="D77" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="E77" s="22">
+        <v>31.16</v>
+      </c>
+      <c r="F77" s="22">
+        <v>31.65</v>
+      </c>
+      <c r="G77" s="22">
+        <v>31.097</v>
+      </c>
+      <c r="H77" s="22">
+        <v>30.455</v>
+      </c>
+      <c r="I77" s="22">
+        <v>31.14</v>
+      </c>
+      <c r="J77" s="27">
+        <v>30.39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="23" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77">
-        <v>1</v>
-      </c>
-      <c r="B77" s="19" t="s">
+      <c r="B78" s="24">
+        <v>43872</v>
+      </c>
+      <c r="C78" s="24">
+        <v>50137</v>
+      </c>
+      <c r="D78" s="24">
+        <v>52811</v>
+      </c>
+      <c r="E78" s="24">
+        <v>54062</v>
+      </c>
+      <c r="F78" s="24">
+        <v>39910</v>
+      </c>
+      <c r="G78" s="24">
+        <v>35794</v>
+      </c>
+      <c r="H78" s="24">
+        <v>20494</v>
+      </c>
+      <c r="I78" s="24">
+        <v>4395</v>
+      </c>
+      <c r="J78" s="28">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="B79" s="24">
+        <v>0</v>
+      </c>
+      <c r="C79" s="24">
+        <v>0</v>
+      </c>
+      <c r="D79" s="24">
+        <v>18</v>
+      </c>
+      <c r="E79" s="24">
+        <v>91</v>
+      </c>
+      <c r="F79" s="24">
+        <v>15578</v>
+      </c>
+      <c r="G79" s="24">
+        <v>20511</v>
+      </c>
+      <c r="H79" s="24">
+        <v>36053</v>
+      </c>
+      <c r="I79" s="24">
+        <v>52368</v>
+      </c>
+      <c r="J79" s="28">
+        <v>55675</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="D77" s="20">
-        <v>40335</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
-      <c r="A78">
-        <v>2</v>
-      </c>
-      <c r="B78" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C78" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D78" s="20">
-        <v>42077</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79">
-        <v>3</v>
-      </c>
-      <c r="B79" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C79" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D79" s="20">
-        <v>41975</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80">
-        <v>4</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C80" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D80" s="20">
-        <v>38629</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81">
-        <v>5</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C81" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D81" s="20">
-        <v>36516</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82">
-        <v>6</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C82" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D82" s="20">
-        <v>38683</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83">
-        <v>7</v>
-      </c>
-      <c r="B83" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D83" s="20">
-        <v>42698</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84">
-        <v>8</v>
-      </c>
-      <c r="B84" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D84" s="20">
-        <v>39131</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
-      <c r="A85">
-        <v>9</v>
-      </c>
-      <c r="B85" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D85" s="20">
-        <v>36044</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86">
+      <c r="B80" s="25">
+        <f>B78+B79</f>
+        <v>43872</v>
+      </c>
+      <c r="C80" s="25">
+        <f>C78+C79</f>
+        <v>50137</v>
+      </c>
+      <c r="D80" s="25">
+        <f>D78+D79</f>
+        <v>52829</v>
+      </c>
+      <c r="E80" s="25">
+        <f>E78+E79</f>
+        <v>54153</v>
+      </c>
+      <c r="F80" s="25">
+        <f>F78+F79</f>
+        <v>55488</v>
+      </c>
+      <c r="G80" s="25">
+        <f>G78+G79</f>
+        <v>56305</v>
+      </c>
+      <c r="H80" s="25">
+        <f>H78+H79</f>
+        <v>56547</v>
+      </c>
+      <c r="I80" s="25">
+        <f>I78+I79</f>
+        <v>56763</v>
+      </c>
+      <c r="J80" s="29">
+        <f>J78+J79</f>
+        <v>56952</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="B81" s="26">
+        <f>B79/B80</f>
+        <v>0</v>
+      </c>
+      <c r="C81" s="26">
+        <f>C79/C80</f>
+        <v>0</v>
+      </c>
+      <c r="D81" s="26">
+        <f>D79/D80</f>
+        <v>0.000340721951958205</v>
+      </c>
+      <c r="E81" s="26">
+        <f>E79/E80</f>
+        <v>0.00168042398389748</v>
+      </c>
+      <c r="F81" s="26">
+        <f>F79/F80</f>
+        <v>0.28074538638985</v>
+      </c>
+      <c r="G81" s="26">
+        <f>G79/G80</f>
+        <v>0.364283811384424</v>
+      </c>
+      <c r="H81" s="26">
+        <f>H79/H80</f>
+        <v>0.637575821882682</v>
+      </c>
+      <c r="I81" s="26">
+        <f>I79/I80</f>
+        <v>0.922572802705988</v>
+      </c>
+      <c r="J81" s="30">
+        <f>J79/J80</f>
+        <v>0.977577609214777</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="23" t="s">
+        <v>257</v>
+      </c>
+      <c r="B82" s="24">
         <v>10</v>
       </c>
-      <c r="B86" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C86" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="D86" s="20">
-        <v>41471</v>
-      </c>
-    </row>
-    <row r="87" spans="4:4">
-      <c r="D87">
-        <f>SUM(D77:D86)/10/1000</f>
-        <v>39.7559</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4">
-      <c r="B89" s="19" t="s">
-        <v>251</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>252</v>
-      </c>
-      <c r="D89" s="19" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
-      <c r="A90">
-        <v>1</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C90" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D90" s="20">
-        <v>38205</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91">
-        <v>2</v>
-      </c>
-      <c r="B91" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C91" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D91" s="20">
-        <v>38344</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92">
-        <v>3</v>
-      </c>
-      <c r="B92" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C92" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D92" s="20">
-        <v>38755</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93">
-        <v>4</v>
-      </c>
-      <c r="B93" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C93" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D93" s="20">
-        <v>41316</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4">
-      <c r="A94">
-        <v>5</v>
-      </c>
-      <c r="B94" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C94" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D94" s="20">
-        <v>40710</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95">
-        <v>6</v>
-      </c>
-      <c r="B95" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C95" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D95" s="20">
-        <v>42358</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96">
-        <v>7</v>
-      </c>
-      <c r="B96" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C96" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D96" s="20">
-        <v>35712</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97">
-        <v>8</v>
-      </c>
-      <c r="B97" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C97" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D97" s="20">
-        <v>38505</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98">
-        <v>9</v>
-      </c>
-      <c r="B98" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C98" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D98" s="20">
-        <v>30665</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99">
+      <c r="C82" s="24">
         <v>10</v>
       </c>
-      <c r="B99" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="C99" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="D99" s="20">
-        <v>33885</v>
-      </c>
-    </row>
-    <row r="100" spans="4:4">
-      <c r="D100">
-        <f>SUM(D90:D99)/10/1000</f>
-        <v>37.8455</v>
-      </c>
+      <c r="D82" s="24">
+        <v>10</v>
+      </c>
+      <c r="E82" s="24">
+        <v>10</v>
+      </c>
+      <c r="F82" s="24">
+        <v>10</v>
+      </c>
+      <c r="G82" s="24">
+        <v>10</v>
+      </c>
+      <c r="H82" s="24">
+        <v>10</v>
+      </c>
+      <c r="I82" s="24">
+        <v>10</v>
+      </c>
+      <c r="J82" s="31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="B83" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="C83" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="D83" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="E83" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F83" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="G83" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="H83" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="I83" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="J83" s="31">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="B84" s="24">
+        <v>0.55</v>
+      </c>
+      <c r="C84" s="24">
+        <v>0.55</v>
+      </c>
+      <c r="D84" s="24">
+        <v>0.55</v>
+      </c>
+      <c r="E84" s="24">
+        <v>0.55</v>
+      </c>
+      <c r="F84" s="24">
+        <v>0.55</v>
+      </c>
+      <c r="G84" s="24">
+        <v>0.55</v>
+      </c>
+      <c r="H84" s="24">
+        <v>0.55</v>
+      </c>
+      <c r="I84" s="24">
+        <v>0.55</v>
+      </c>
+      <c r="J84" s="31">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="B85" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C85" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="D85" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="E85" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="F85" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G85" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="H85" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="I85" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="J85" s="31">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
+      <c r="A86" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="B86" s="24">
+        <v>10</v>
+      </c>
+      <c r="C86" s="24">
+        <v>10</v>
+      </c>
+      <c r="D86" s="24">
+        <v>10</v>
+      </c>
+      <c r="E86" s="24">
+        <v>10</v>
+      </c>
+      <c r="F86" s="24">
+        <v>10</v>
+      </c>
+      <c r="G86" s="24">
+        <v>10</v>
+      </c>
+      <c r="H86" s="24">
+        <v>10</v>
+      </c>
+      <c r="I86" s="24">
+        <v>10</v>
+      </c>
+      <c r="J86" s="31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="B87" s="24">
+        <v>250</v>
+      </c>
+      <c r="C87" s="24">
+        <v>250</v>
+      </c>
+      <c r="D87" s="24">
+        <v>250</v>
+      </c>
+      <c r="E87" s="24">
+        <v>250</v>
+      </c>
+      <c r="F87" s="24">
+        <v>250</v>
+      </c>
+      <c r="G87" s="24">
+        <v>250</v>
+      </c>
+      <c r="H87" s="24">
+        <v>250</v>
+      </c>
+      <c r="I87" s="24">
+        <v>250</v>
+      </c>
+      <c r="J87" s="31">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
+      <c r="A88" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="B88" s="24">
+        <v>1.1</v>
+      </c>
+      <c r="C88" s="24">
+        <v>1.1</v>
+      </c>
+      <c r="D88" s="24">
+        <v>1.1</v>
+      </c>
+      <c r="E88" s="24">
+        <v>1.1</v>
+      </c>
+      <c r="F88" s="24">
+        <v>1.1</v>
+      </c>
+      <c r="G88" s="24">
+        <v>1.1</v>
+      </c>
+      <c r="H88" s="24">
+        <v>1.1</v>
+      </c>
+      <c r="I88" s="24">
+        <v>1.1</v>
+      </c>
+      <c r="J88" s="31">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
+      <c r="A89" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="B89" s="24">
+        <v>863</v>
+      </c>
+      <c r="C89" s="24">
+        <v>863</v>
+      </c>
+      <c r="D89" s="24">
+        <v>863</v>
+      </c>
+      <c r="E89" s="24">
+        <v>863</v>
+      </c>
+      <c r="F89" s="24">
+        <v>863</v>
+      </c>
+      <c r="G89" s="24">
+        <v>863</v>
+      </c>
+      <c r="H89" s="24">
+        <v>863</v>
+      </c>
+      <c r="I89" s="24">
+        <v>863</v>
+      </c>
+      <c r="J89" s="24">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
+      <c r="A90" s="23"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="24"/>
+      <c r="J90" s="28"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="A91" s="23"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+      <c r="J91" s="28"/>
+    </row>
+    <row r="92" spans="1:10">
+      <c r="A92" s="8"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="24"/>
+      <c r="J92" s="28"/>
+    </row>
+    <row r="93" spans="1:10">
+      <c r="A93" s="8"/>
+      <c r="B93" s="9"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="17"/>
+    </row>
+    <row r="94" spans="1:10">
+      <c r="A94" s="8"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
+      <c r="I94" s="9"/>
+      <c r="J94" s="17"/>
+    </row>
+    <row r="95" spans="1:10">
+      <c r="A95" s="8"/>
+      <c r="B95" s="9"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="17"/>
+    </row>
+    <row r="96" spans="1:10">
+      <c r="A96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="17"/>
+    </row>
+    <row r="97" spans="1:10">
+      <c r="A97" s="8"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="17"/>
+    </row>
+    <row r="98" spans="1:10">
+      <c r="A98" s="8"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="12"/>
+      <c r="J98" s="17"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="A99" s="8"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="12"/>
+      <c r="J99" s="17"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="A100" s="8"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="9"/>
+      <c r="H100" s="9"/>
+      <c r="I100" s="12"/>
+      <c r="J100" s="17"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="A101" s="8"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
+      <c r="I101" s="9"/>
+      <c r="J101" s="17"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="A102" s="8"/>
+      <c r="B102" s="9"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="17"/>
+    </row>
+    <row r="103" spans="1:10">
+      <c r="A103" s="8"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="17"/>
+    </row>
+    <row r="104" spans="1:10">
+      <c r="A104" s="8"/>
+      <c r="B104" s="9"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="17"/>
+    </row>
+    <row r="105" spans="1:10">
+      <c r="A105" s="8"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="17"/>
+    </row>
+    <row r="106" spans="1:10">
+      <c r="A106" s="8"/>
+      <c r="B106" s="9"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+      <c r="H106" s="9"/>
+      <c r="I106" s="9"/>
+      <c r="J106" s="17"/>
+    </row>
+    <row r="107" spans="1:10">
+      <c r="A107" s="8"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9"/>
+      <c r="I107" s="9"/>
+      <c r="J107" s="17"/>
+    </row>
+    <row r="108" ht="13.5" spans="1:10">
+      <c r="A108" s="10"/>
+      <c r="B108" s="11"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="11"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Y1:AA1"/>
@@ -8510,6 +8976,8 @@
     <mergeCell ref="N37:P37"/>
     <mergeCell ref="B38:J38"/>
     <mergeCell ref="O38:W38"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="B75:J75"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Updated files for FDR analysis
</commit_message>
<xml_diff>
--- a/utils/FER_S1G_Analysis.xlsx
+++ b/utils/FER_S1G_Analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="266">
   <si>
     <t>CFO: 0 ppm | SFO: 0 ppm</t>
   </si>
@@ -772,9 +772,6 @@
     <t>AVG SNR [dB]</t>
   </si>
   <si>
-    <t>35,095?</t>
-  </si>
-  <si>
     <t>SUCCSESS</t>
   </si>
   <si>
@@ -809,6 +806,12 @@
   </si>
   <si>
     <t>Center Freq. [MHz]</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>30k</t>
   </si>
 </sst>
 </file>
@@ -816,10 +819,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -838,8 +841,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -860,24 +864,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -891,36 +925,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -928,27 +932,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -967,7 +962,7 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -976,7 +971,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -991,25 +994,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,13 +1018,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1039,37 +1054,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1087,7 +1072,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1099,79 +1156,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1334,17 +1337,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1354,6 +1351,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1384,11 +1396,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1407,181 +1434,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1657,9 +1660,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1669,13 +1669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1997,10 +1991,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AS108"/>
+  <dimension ref="A1:AS122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="C101" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -2022,13 +2016,6 @@
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1"/>
-      <c r="R1"/>
-      <c r="S1"/>
-      <c r="T1"/>
-      <c r="U1"/>
-      <c r="V1"/>
-      <c r="W1"/>
       <c r="Y1" s="1" t="s">
         <v>1</v>
       </c>
@@ -8305,68 +8292,68 @@
         <v>251</v>
       </c>
       <c r="B77" s="21">
-        <v>30.219</v>
+        <v>20.99</v>
       </c>
       <c r="C77" s="22">
-        <v>30.25</v>
-      </c>
-      <c r="D77" s="22" t="s">
-        <v>252</v>
+        <v>21.89</v>
+      </c>
+      <c r="D77" s="22">
+        <v>25.84</v>
       </c>
       <c r="E77" s="22">
-        <v>31.16</v>
+        <v>22.19</v>
       </c>
       <c r="F77" s="22">
-        <v>31.65</v>
+        <v>25.21</v>
       </c>
       <c r="G77" s="22">
-        <v>31.097</v>
+        <v>25.69</v>
       </c>
       <c r="H77" s="22">
-        <v>30.455</v>
+        <v>26.12</v>
       </c>
       <c r="I77" s="22">
-        <v>31.14</v>
-      </c>
-      <c r="J77" s="27">
-        <v>30.39</v>
+        <v>31.85</v>
+      </c>
+      <c r="J77" s="26">
+        <v>31.66</v>
       </c>
     </row>
     <row r="78" spans="1:10">
       <c r="A78" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B78" s="24">
-        <v>43872</v>
+        <v>43827</v>
       </c>
       <c r="C78" s="24">
-        <v>50137</v>
+        <v>50151</v>
       </c>
       <c r="D78" s="24">
-        <v>52811</v>
+        <v>52738</v>
       </c>
       <c r="E78" s="24">
-        <v>54062</v>
+        <v>53927</v>
       </c>
       <c r="F78" s="24">
-        <v>39910</v>
+        <v>36661</v>
       </c>
       <c r="G78" s="24">
-        <v>35794</v>
+        <v>28487</v>
       </c>
       <c r="H78" s="24">
-        <v>20494</v>
+        <v>15367</v>
       </c>
       <c r="I78" s="24">
-        <v>4395</v>
-      </c>
-      <c r="J78" s="28">
-        <v>1277</v>
+        <v>4292</v>
+      </c>
+      <c r="J78" s="27">
+        <v>1793</v>
       </c>
     </row>
     <row r="79" spans="1:10">
       <c r="A79" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B79" s="24">
         <v>0</v>
@@ -8375,112 +8362,112 @@
         <v>0</v>
       </c>
       <c r="D79" s="24">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E79" s="24">
-        <v>91</v>
+        <v>198</v>
       </c>
       <c r="F79" s="24">
-        <v>15578</v>
+        <v>18941</v>
       </c>
       <c r="G79" s="24">
-        <v>20511</v>
+        <v>27769</v>
       </c>
       <c r="H79" s="24">
-        <v>36053</v>
+        <v>41171</v>
       </c>
       <c r="I79" s="24">
-        <v>52368</v>
-      </c>
-      <c r="J79" s="28">
-        <v>55675</v>
+        <v>52483</v>
+      </c>
+      <c r="J79" s="27">
+        <v>55121</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="23" t="s">
-        <v>255</v>
-      </c>
-      <c r="B80" s="25">
-        <f>B78+B79</f>
-        <v>43872</v>
-      </c>
-      <c r="C80" s="25">
-        <f>C78+C79</f>
-        <v>50137</v>
-      </c>
-      <c r="D80" s="25">
-        <f>D78+D79</f>
-        <v>52829</v>
-      </c>
-      <c r="E80" s="25">
-        <f>E78+E79</f>
-        <v>54153</v>
-      </c>
-      <c r="F80" s="25">
-        <f>F78+F79</f>
-        <v>55488</v>
-      </c>
-      <c r="G80" s="25">
-        <f>G78+G79</f>
-        <v>56305</v>
-      </c>
-      <c r="H80" s="25">
-        <f>H78+H79</f>
-        <v>56547</v>
-      </c>
-      <c r="I80" s="25">
-        <f>I78+I79</f>
-        <v>56763</v>
-      </c>
-      <c r="J80" s="29">
-        <f>J78+J79</f>
-        <v>56952</v>
+        <v>254</v>
+      </c>
+      <c r="B80" s="24">
+        <f t="shared" ref="B80:J80" si="0">B78+B79</f>
+        <v>43827</v>
+      </c>
+      <c r="C80" s="24">
+        <f t="shared" si="0"/>
+        <v>50151</v>
+      </c>
+      <c r="D80" s="24">
+        <f t="shared" si="0"/>
+        <v>52762</v>
+      </c>
+      <c r="E80" s="24">
+        <f t="shared" si="0"/>
+        <v>54125</v>
+      </c>
+      <c r="F80" s="24">
+        <f t="shared" si="0"/>
+        <v>55602</v>
+      </c>
+      <c r="G80" s="24">
+        <f t="shared" si="0"/>
+        <v>56256</v>
+      </c>
+      <c r="H80" s="24">
+        <f t="shared" si="0"/>
+        <v>56538</v>
+      </c>
+      <c r="I80" s="24">
+        <f t="shared" si="0"/>
+        <v>56775</v>
+      </c>
+      <c r="J80" s="27">
+        <f t="shared" si="0"/>
+        <v>56914</v>
       </c>
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="23" t="s">
-        <v>256</v>
-      </c>
-      <c r="B81" s="26">
-        <f>B79/B80</f>
+        <v>255</v>
+      </c>
+      <c r="B81" s="25">
+        <f t="shared" ref="B81:J81" si="1">B79/B80</f>
         <v>0</v>
       </c>
-      <c r="C81" s="26">
-        <f>C79/C80</f>
+      <c r="C81" s="25">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D81" s="26">
-        <f>D79/D80</f>
-        <v>0.000340721951958205</v>
-      </c>
-      <c r="E81" s="26">
-        <f>E79/E80</f>
-        <v>0.00168042398389748</v>
-      </c>
-      <c r="F81" s="26">
-        <f>F79/F80</f>
-        <v>0.28074538638985</v>
-      </c>
-      <c r="G81" s="26">
-        <f>G79/G80</f>
-        <v>0.364283811384424</v>
-      </c>
-      <c r="H81" s="26">
-        <f>H79/H80</f>
-        <v>0.637575821882682</v>
-      </c>
-      <c r="I81" s="26">
-        <f>I79/I80</f>
-        <v>0.922572802705988</v>
-      </c>
-      <c r="J81" s="30">
-        <f>J79/J80</f>
-        <v>0.977577609214777</v>
+      <c r="D81" s="25">
+        <f t="shared" si="1"/>
+        <v>0.000454872825139305</v>
+      </c>
+      <c r="E81" s="25">
+        <f t="shared" si="1"/>
+        <v>0.00365819861431871</v>
+      </c>
+      <c r="F81" s="25">
+        <f t="shared" si="1"/>
+        <v>0.340653213913169</v>
+      </c>
+      <c r="G81" s="25">
+        <f t="shared" si="1"/>
+        <v>0.49361845847554</v>
+      </c>
+      <c r="H81" s="25">
+        <f t="shared" si="1"/>
+        <v>0.728200502317026</v>
+      </c>
+      <c r="I81" s="25">
+        <f t="shared" si="1"/>
+        <v>0.924403346543373</v>
+      </c>
+      <c r="J81" s="28">
+        <f t="shared" si="1"/>
+        <v>0.96849632779281</v>
       </c>
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B82" s="24">
         <v>10</v>
@@ -8506,13 +8493,13 @@
       <c r="I82" s="24">
         <v>10</v>
       </c>
-      <c r="J82" s="31">
+      <c r="J82" s="27">
         <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B83" s="24">
         <v>0.6</v>
@@ -8538,13 +8525,13 @@
       <c r="I83" s="24">
         <v>0.6</v>
       </c>
-      <c r="J83" s="31">
+      <c r="J83" s="27">
         <v>0.6</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B84" s="24">
         <v>0.55</v>
@@ -8570,13 +8557,13 @@
       <c r="I84" s="24">
         <v>0.55</v>
       </c>
-      <c r="J84" s="31">
+      <c r="J84" s="27">
         <v>0.55</v>
       </c>
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B85" s="24">
         <v>0.3</v>
@@ -8602,13 +8589,13 @@
       <c r="I85" s="24">
         <v>0.3</v>
       </c>
-      <c r="J85" s="31">
+      <c r="J85" s="27">
         <v>0.3</v>
       </c>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B86" s="24">
         <v>10</v>
@@ -8634,13 +8621,13 @@
       <c r="I86" s="24">
         <v>10</v>
       </c>
-      <c r="J86" s="31">
+      <c r="J86" s="27">
         <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B87" s="24">
         <v>250</v>
@@ -8666,13 +8653,13 @@
       <c r="I87" s="24">
         <v>250</v>
       </c>
-      <c r="J87" s="31">
+      <c r="J87" s="27">
         <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B88" s="24">
         <v>1.1</v>
@@ -8698,13 +8685,13 @@
       <c r="I88" s="24">
         <v>1.1</v>
       </c>
-      <c r="J88" s="31">
+      <c r="J88" s="27">
         <v>1.1</v>
       </c>
     </row>
     <row r="89" spans="1:10">
       <c r="A89" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B89" s="24">
         <v>863</v>
@@ -8734,7 +8721,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" ht="13.5" spans="1:10">
       <c r="A90" s="23"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -8744,163 +8731,415 @@
       <c r="G90" s="24"/>
       <c r="H90" s="24"/>
       <c r="I90" s="24"/>
-      <c r="J90" s="28"/>
+      <c r="J90" s="27"/>
     </row>
     <row r="91" spans="1:10">
       <c r="A91" s="23"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24"/>
-      <c r="H91" s="24"/>
-      <c r="I91" s="24"/>
-      <c r="J91" s="28"/>
+      <c r="B91" s="22">
+        <v>34.82</v>
+      </c>
+      <c r="C91" s="22">
+        <v>33.43</v>
+      </c>
+      <c r="D91" s="22">
+        <v>35.54</v>
+      </c>
+      <c r="E91" s="22">
+        <v>34.29</v>
+      </c>
+      <c r="F91" s="22">
+        <v>33.5</v>
+      </c>
+      <c r="G91" s="22">
+        <v>33.64</v>
+      </c>
+      <c r="H91" s="22">
+        <v>32.8</v>
+      </c>
+      <c r="I91" s="22">
+        <v>34.74</v>
+      </c>
+      <c r="J91" s="22">
+        <v>34.39</v>
+      </c>
     </row>
     <row r="92" spans="1:10">
       <c r="A92" s="8"/>
-      <c r="B92" s="9"/>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
-      <c r="E92" s="9"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="24"/>
-      <c r="H92" s="24"/>
-      <c r="I92" s="24"/>
-      <c r="J92" s="28"/>
+      <c r="B92" s="24">
+        <v>7184</v>
+      </c>
+      <c r="C92" s="24">
+        <v>7331</v>
+      </c>
+      <c r="D92" s="24">
+        <v>7387</v>
+      </c>
+      <c r="E92" s="24">
+        <v>7417</v>
+      </c>
+      <c r="F92" s="24">
+        <v>7429</v>
+      </c>
+      <c r="G92" s="24">
+        <v>6831</v>
+      </c>
+      <c r="H92" s="24">
+        <v>6994</v>
+      </c>
+      <c r="I92" s="24">
+        <v>6037</v>
+      </c>
+      <c r="J92" s="24">
+        <v>2866</v>
+      </c>
     </row>
     <row r="93" spans="1:10">
       <c r="A93" s="8"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="9"/>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9"/>
-      <c r="F93" s="9"/>
-      <c r="G93" s="9"/>
-      <c r="H93" s="9"/>
-      <c r="I93" s="9"/>
-      <c r="J93" s="17"/>
+      <c r="B93" s="24">
+        <v>0</v>
+      </c>
+      <c r="C93" s="24">
+        <v>3</v>
+      </c>
+      <c r="D93" s="24">
+        <v>0</v>
+      </c>
+      <c r="E93" s="24">
+        <v>6</v>
+      </c>
+      <c r="F93" s="24">
+        <v>1</v>
+      </c>
+      <c r="G93" s="24">
+        <v>632</v>
+      </c>
+      <c r="H93" s="24">
+        <v>427</v>
+      </c>
+      <c r="I93" s="24">
+        <v>1420</v>
+      </c>
+      <c r="J93" s="24">
+        <v>4622</v>
+      </c>
     </row>
     <row r="94" spans="1:10">
       <c r="A94" s="8"/>
-      <c r="B94" s="9"/>
-      <c r="C94" s="9"/>
-      <c r="D94" s="9"/>
-      <c r="E94" s="9"/>
-      <c r="F94" s="9"/>
-      <c r="G94" s="9"/>
-      <c r="H94" s="9"/>
-      <c r="I94" s="9"/>
-      <c r="J94" s="17"/>
+      <c r="B94" s="24">
+        <f t="shared" ref="B94:J94" si="2">B92+B93</f>
+        <v>7184</v>
+      </c>
+      <c r="C94" s="24">
+        <f t="shared" si="2"/>
+        <v>7334</v>
+      </c>
+      <c r="D94" s="24">
+        <f t="shared" si="2"/>
+        <v>7387</v>
+      </c>
+      <c r="E94" s="24">
+        <f t="shared" si="2"/>
+        <v>7423</v>
+      </c>
+      <c r="F94" s="24">
+        <f t="shared" si="2"/>
+        <v>7430</v>
+      </c>
+      <c r="G94" s="24">
+        <f t="shared" si="2"/>
+        <v>7463</v>
+      </c>
+      <c r="H94" s="24">
+        <f t="shared" si="2"/>
+        <v>7421</v>
+      </c>
+      <c r="I94" s="24">
+        <f t="shared" si="2"/>
+        <v>7457</v>
+      </c>
+      <c r="J94" s="24">
+        <f t="shared" si="2"/>
+        <v>7488</v>
+      </c>
     </row>
     <row r="95" spans="1:10">
       <c r="A95" s="8"/>
-      <c r="B95" s="9"/>
-      <c r="C95" s="9"/>
-      <c r="D95" s="9"/>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="9"/>
-      <c r="H95" s="9"/>
-      <c r="I95" s="9"/>
-      <c r="J95" s="17"/>
+      <c r="B95" s="25">
+        <f t="shared" ref="B95:J95" si="3">B93/B94</f>
+        <v>0</v>
+      </c>
+      <c r="C95" s="25">
+        <f t="shared" si="3"/>
+        <v>0.000409053722388874</v>
+      </c>
+      <c r="D95" s="25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E95" s="25">
+        <f t="shared" si="3"/>
+        <v>0.000808298531591001</v>
+      </c>
+      <c r="F95" s="25">
+        <f t="shared" si="3"/>
+        <v>0.000134589502018843</v>
+      </c>
+      <c r="G95" s="25">
+        <f t="shared" si="3"/>
+        <v>0.0846844432533834</v>
+      </c>
+      <c r="H95" s="25">
+        <f t="shared" si="3"/>
+        <v>0.0575394151731573</v>
+      </c>
+      <c r="I95" s="25">
+        <f t="shared" si="3"/>
+        <v>0.190425103929194</v>
+      </c>
+      <c r="J95" s="25">
+        <f t="shared" si="3"/>
+        <v>0.617254273504274</v>
+      </c>
     </row>
     <row r="96" spans="1:10">
       <c r="A96" s="8"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="9"/>
-      <c r="D96" s="9"/>
-      <c r="E96" s="9"/>
-      <c r="F96" s="9"/>
-      <c r="G96" s="9"/>
-      <c r="H96" s="9"/>
-      <c r="I96" s="9"/>
-      <c r="J96" s="17"/>
+      <c r="B96" s="24">
+        <v>10</v>
+      </c>
+      <c r="C96" s="24">
+        <v>10</v>
+      </c>
+      <c r="D96" s="24">
+        <v>10</v>
+      </c>
+      <c r="E96" s="24">
+        <v>10</v>
+      </c>
+      <c r="F96" s="24">
+        <v>10</v>
+      </c>
+      <c r="G96" s="24">
+        <v>10</v>
+      </c>
+      <c r="H96" s="24">
+        <v>10</v>
+      </c>
+      <c r="I96" s="24">
+        <v>10</v>
+      </c>
+      <c r="J96" s="24">
+        <v>10</v>
+      </c>
     </row>
     <row r="97" spans="1:10">
       <c r="A97" s="8"/>
-      <c r="B97" s="9"/>
-      <c r="C97" s="9"/>
-      <c r="D97" s="9"/>
-      <c r="E97" s="9"/>
-      <c r="F97" s="9"/>
-      <c r="G97" s="12"/>
-      <c r="H97" s="12"/>
-      <c r="I97" s="12"/>
-      <c r="J97" s="17"/>
+      <c r="B97" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="C97" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="D97" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="E97" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="F97" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="G97" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="H97" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="I97" s="24">
+        <v>0.75</v>
+      </c>
+      <c r="J97" s="24">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="98" spans="1:10">
       <c r="A98" s="8"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9"/>
-      <c r="E98" s="9"/>
-      <c r="F98" s="9"/>
-      <c r="G98" s="9"/>
-      <c r="H98" s="12"/>
-      <c r="I98" s="12"/>
-      <c r="J98" s="17"/>
+      <c r="B98" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="C98" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="D98" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="E98" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="F98" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="G98" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="H98" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="I98" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="J98" s="24">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="99" spans="1:10">
       <c r="A99" s="8"/>
-      <c r="B99" s="9"/>
-      <c r="C99" s="9"/>
-      <c r="D99" s="9"/>
-      <c r="E99" s="9"/>
-      <c r="F99" s="9"/>
-      <c r="G99" s="9"/>
-      <c r="H99" s="12"/>
-      <c r="I99" s="12"/>
-      <c r="J99" s="17"/>
+      <c r="B99" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C99" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="D99" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="E99" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="F99" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G99" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="H99" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="I99" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="J99" s="24">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="100" spans="1:10">
       <c r="A100" s="8"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
-      <c r="E100" s="9"/>
-      <c r="F100" s="9"/>
-      <c r="G100" s="9"/>
-      <c r="H100" s="9"/>
-      <c r="I100" s="12"/>
-      <c r="J100" s="17"/>
+      <c r="B100" s="24">
+        <v>10</v>
+      </c>
+      <c r="C100" s="24">
+        <v>10</v>
+      </c>
+      <c r="D100" s="24">
+        <v>10</v>
+      </c>
+      <c r="E100" s="24">
+        <v>10</v>
+      </c>
+      <c r="F100" s="24">
+        <v>10</v>
+      </c>
+      <c r="G100" s="24">
+        <v>10</v>
+      </c>
+      <c r="H100" s="24">
+        <v>10</v>
+      </c>
+      <c r="I100" s="24">
+        <v>10</v>
+      </c>
+      <c r="J100" s="24">
+        <v>10</v>
+      </c>
     </row>
     <row r="101" spans="1:10">
       <c r="A101" s="8"/>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
-      <c r="D101" s="9"/>
-      <c r="E101" s="9"/>
-      <c r="F101" s="9"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="9"/>
-      <c r="I101" s="9"/>
-      <c r="J101" s="17"/>
+      <c r="B101" s="24">
+        <v>250</v>
+      </c>
+      <c r="C101" s="24">
+        <v>250</v>
+      </c>
+      <c r="D101" s="24">
+        <v>250</v>
+      </c>
+      <c r="E101" s="24">
+        <v>250</v>
+      </c>
+      <c r="F101" s="24">
+        <v>250</v>
+      </c>
+      <c r="G101" s="24">
+        <v>250</v>
+      </c>
+      <c r="H101" s="24">
+        <v>250</v>
+      </c>
+      <c r="I101" s="24">
+        <v>250</v>
+      </c>
+      <c r="J101" s="24">
+        <v>250</v>
+      </c>
     </row>
     <row r="102" spans="1:10">
       <c r="A102" s="8"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="9"/>
-      <c r="D102" s="9"/>
-      <c r="E102" s="9"/>
-      <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="9"/>
-      <c r="I102" s="9"/>
-      <c r="J102" s="17"/>
+      <c r="B102" s="24">
+        <v>0</v>
+      </c>
+      <c r="C102" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="D102" s="24">
+        <v>0</v>
+      </c>
+      <c r="E102" s="24">
+        <v>0</v>
+      </c>
+      <c r="F102" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="G102" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="H102" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="I102" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="J102" s="24" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="103" spans="1:10">
       <c r="A103" s="8"/>
-      <c r="B103" s="9"/>
-      <c r="C103" s="9"/>
-      <c r="D103" s="9"/>
-      <c r="E103" s="9"/>
-      <c r="F103" s="9"/>
-      <c r="G103" s="9"/>
-      <c r="H103" s="9"/>
-      <c r="I103" s="9"/>
-      <c r="J103" s="17"/>
+      <c r="B103" s="24">
+        <v>863</v>
+      </c>
+      <c r="C103" s="24">
+        <v>863</v>
+      </c>
+      <c r="D103" s="24">
+        <v>863</v>
+      </c>
+      <c r="E103" s="24">
+        <v>863</v>
+      </c>
+      <c r="F103" s="24">
+        <v>863</v>
+      </c>
+      <c r="G103" s="24">
+        <v>863</v>
+      </c>
+      <c r="H103" s="24">
+        <v>863</v>
+      </c>
+      <c r="I103" s="24">
+        <v>863</v>
+      </c>
+      <c r="J103" s="24">
+        <v>863</v>
+      </c>
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="8"/>
@@ -8961,6 +9200,402 @@
       <c r="H108" s="11"/>
       <c r="I108" s="11"/>
       <c r="J108" s="18"/>
+    </row>
+    <row r="109" ht="13.5"/>
+    <row r="110" spans="2:10">
+      <c r="B110" s="22">
+        <v>28</v>
+      </c>
+      <c r="C110" s="22">
+        <v>28.36</v>
+      </c>
+      <c r="D110" s="22">
+        <v>28.75</v>
+      </c>
+      <c r="E110" s="22">
+        <v>33.61</v>
+      </c>
+      <c r="F110" s="22">
+        <v>30.44</v>
+      </c>
+      <c r="G110" s="22">
+        <v>30.33</v>
+      </c>
+      <c r="H110" s="22">
+        <v>30.16</v>
+      </c>
+      <c r="I110" s="22">
+        <v>30</v>
+      </c>
+      <c r="J110" s="22">
+        <v>33.75</v>
+      </c>
+    </row>
+    <row r="111" spans="2:10">
+      <c r="B111" s="24">
+        <v>7183</v>
+      </c>
+      <c r="C111" s="24">
+        <v>7323</v>
+      </c>
+      <c r="D111" s="24">
+        <v>7389</v>
+      </c>
+      <c r="E111" s="24">
+        <v>7425</v>
+      </c>
+      <c r="F111" s="24">
+        <v>7453</v>
+      </c>
+      <c r="G111" s="24">
+        <v>7469</v>
+      </c>
+      <c r="H111" s="24">
+        <v>7417</v>
+      </c>
+      <c r="I111" s="24">
+        <v>7187</v>
+      </c>
+      <c r="J111" s="24">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="112" spans="2:10">
+      <c r="B112" s="24">
+        <v>0</v>
+      </c>
+      <c r="C112" s="24">
+        <v>1</v>
+      </c>
+      <c r="D112" s="24">
+        <v>1</v>
+      </c>
+      <c r="E112" s="24">
+        <v>5</v>
+      </c>
+      <c r="F112" s="24">
+        <v>0</v>
+      </c>
+      <c r="G112" s="24">
+        <v>11</v>
+      </c>
+      <c r="H112" s="24">
+        <v>32</v>
+      </c>
+      <c r="I112" s="24">
+        <v>267</v>
+      </c>
+      <c r="J112" s="24">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10">
+      <c r="B113" s="24">
+        <f>B111+B112</f>
+        <v>7183</v>
+      </c>
+      <c r="C113" s="24">
+        <f>C111+C112</f>
+        <v>7324</v>
+      </c>
+      <c r="D113" s="24">
+        <f>D111+D112</f>
+        <v>7390</v>
+      </c>
+      <c r="E113" s="24">
+        <f>E111+E112</f>
+        <v>7430</v>
+      </c>
+      <c r="F113" s="24">
+        <f>F111+F112</f>
+        <v>7453</v>
+      </c>
+      <c r="G113" s="24">
+        <f>G111+G112</f>
+        <v>7480</v>
+      </c>
+      <c r="H113" s="24">
+        <f t="shared" ref="H113:J113" si="4">H111+H112</f>
+        <v>7449</v>
+      </c>
+      <c r="I113" s="24">
+        <f t="shared" si="4"/>
+        <v>7454</v>
+      </c>
+      <c r="J113" s="24">
+        <f t="shared" si="4"/>
+        <v>7466</v>
+      </c>
+    </row>
+    <row r="114" spans="2:10">
+      <c r="B114" s="25">
+        <f>B112/B113</f>
+        <v>0</v>
+      </c>
+      <c r="C114" s="25">
+        <f>C112/C113</f>
+        <v>0.000136537411250683</v>
+      </c>
+      <c r="D114" s="25">
+        <f>D112/D113</f>
+        <v>0.00013531799729364</v>
+      </c>
+      <c r="E114" s="25">
+        <f>E112/E113</f>
+        <v>0.000672947510094213</v>
+      </c>
+      <c r="F114" s="25">
+        <f>F112/F113</f>
+        <v>0</v>
+      </c>
+      <c r="G114" s="25">
+        <f>G112/G113</f>
+        <v>0.00147058823529412</v>
+      </c>
+      <c r="H114" s="25">
+        <f t="shared" ref="H114:J114" si="5">H112/H113</f>
+        <v>0.00429587864142838</v>
+      </c>
+      <c r="I114" s="25">
+        <f t="shared" si="5"/>
+        <v>0.0358196941239603</v>
+      </c>
+      <c r="J114" s="25">
+        <f t="shared" si="5"/>
+        <v>0.142780605411197</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10">
+      <c r="B115" s="24">
+        <v>10</v>
+      </c>
+      <c r="C115" s="24">
+        <v>10</v>
+      </c>
+      <c r="D115" s="24">
+        <v>10</v>
+      </c>
+      <c r="E115" s="24">
+        <v>10</v>
+      </c>
+      <c r="F115" s="24">
+        <v>10</v>
+      </c>
+      <c r="G115" s="24">
+        <v>10</v>
+      </c>
+      <c r="H115" s="24">
+        <v>10</v>
+      </c>
+      <c r="I115" s="24">
+        <v>10</v>
+      </c>
+      <c r="J115" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="2:10">
+      <c r="B116" s="24">
+        <v>50</v>
+      </c>
+      <c r="C116" s="24">
+        <v>50</v>
+      </c>
+      <c r="D116" s="24">
+        <v>50</v>
+      </c>
+      <c r="E116" s="24">
+        <v>50</v>
+      </c>
+      <c r="F116" s="24">
+        <v>50</v>
+      </c>
+      <c r="G116" s="24">
+        <v>50</v>
+      </c>
+      <c r="H116" s="24">
+        <v>50</v>
+      </c>
+      <c r="I116" s="24">
+        <v>60</v>
+      </c>
+      <c r="J116" s="24">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="117" spans="2:10">
+      <c r="B117" s="24">
+        <v>30</v>
+      </c>
+      <c r="C117" s="24">
+        <v>30</v>
+      </c>
+      <c r="D117" s="24">
+        <v>30</v>
+      </c>
+      <c r="E117" s="24">
+        <v>40</v>
+      </c>
+      <c r="F117" s="24">
+        <v>40</v>
+      </c>
+      <c r="G117" s="24">
+        <v>40</v>
+      </c>
+      <c r="H117" s="24">
+        <v>40</v>
+      </c>
+      <c r="I117" s="24">
+        <v>40</v>
+      </c>
+      <c r="J117" s="24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="118" spans="2:10">
+      <c r="B118" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="C118" s="24">
+        <v>30</v>
+      </c>
+      <c r="D118" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="E118" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="F118" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="G118" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="H118" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="I118" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="J118" s="24">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="119" spans="2:10">
+      <c r="B119" s="24">
+        <v>10</v>
+      </c>
+      <c r="C119" s="24">
+        <v>10</v>
+      </c>
+      <c r="D119" s="24">
+        <v>10</v>
+      </c>
+      <c r="E119" s="24">
+        <v>10</v>
+      </c>
+      <c r="F119" s="24">
+        <v>10</v>
+      </c>
+      <c r="G119" s="24">
+        <v>10</v>
+      </c>
+      <c r="H119" s="24">
+        <v>10</v>
+      </c>
+      <c r="I119" s="24">
+        <v>10</v>
+      </c>
+      <c r="J119" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="2:10">
+      <c r="B120" s="24">
+        <v>250</v>
+      </c>
+      <c r="C120" s="24">
+        <v>250</v>
+      </c>
+      <c r="D120" s="24">
+        <v>250</v>
+      </c>
+      <c r="E120" s="24">
+        <v>250</v>
+      </c>
+      <c r="F120" s="24">
+        <v>250</v>
+      </c>
+      <c r="G120" s="24">
+        <v>250</v>
+      </c>
+      <c r="H120" s="24">
+        <v>250</v>
+      </c>
+      <c r="I120" s="24">
+        <v>250</v>
+      </c>
+      <c r="J120" s="24">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="121" spans="2:10">
+      <c r="B121" s="24">
+        <v>0</v>
+      </c>
+      <c r="C121" s="24">
+        <v>0</v>
+      </c>
+      <c r="D121" s="24">
+        <v>0</v>
+      </c>
+      <c r="E121" s="24">
+        <v>0</v>
+      </c>
+      <c r="F121" s="24">
+        <v>0</v>
+      </c>
+      <c r="G121" s="24">
+        <v>0</v>
+      </c>
+      <c r="H121" s="24">
+        <v>0</v>
+      </c>
+      <c r="I121" s="24">
+        <v>0</v>
+      </c>
+      <c r="J121" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="2:10">
+      <c r="B122" s="24">
+        <v>863</v>
+      </c>
+      <c r="C122" s="24">
+        <v>863</v>
+      </c>
+      <c r="D122" s="24">
+        <v>863</v>
+      </c>
+      <c r="E122" s="24">
+        <v>863</v>
+      </c>
+      <c r="F122" s="24">
+        <v>863</v>
+      </c>
+      <c r="G122" s="24">
+        <v>863</v>
+      </c>
+      <c r="H122" s="24">
+        <v>863</v>
+      </c>
+      <c r="I122" s="24">
+        <v>863</v>
+      </c>
+      <c r="J122" s="24">
+        <v>863</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>